<commit_message>
Updating attendance files 10th feb
</commit_message>
<xml_diff>
--- a/attendance-files/LAB/LAB (F) Attendance Sheet.xlsx
+++ b/attendance-files/LAB/LAB (F) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="181">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>2024PGP011</t>
@@ -1662,7 +1665,9 @@
       <c r="I7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="30"/>
+      <c r="J7" s="29" t="s">
+        <v>22</v>
+      </c>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
       <c r="M7" s="30"/>
@@ -1687,10 +1692,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>9</v>
@@ -1737,10 +1742,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>9</v>
@@ -1787,10 +1792,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>9</v>
@@ -1837,10 +1842,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>9</v>
@@ -1887,10 +1892,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>9</v>
@@ -1937,10 +1942,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>9</v>
@@ -1987,10 +1992,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>9</v>
@@ -2037,10 +2042,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>9</v>
@@ -2087,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>9</v>
@@ -2137,10 +2142,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>9</v>
@@ -2187,10 +2192,10 @@
         <v>12</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>9</v>
@@ -2237,10 +2242,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>9</v>
@@ -2287,10 +2292,10 @@
         <v>14</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>9</v>
@@ -2337,10 +2342,10 @@
         <v>15</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>9</v>
@@ -2387,10 +2392,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>9</v>
@@ -2437,10 +2442,10 @@
         <v>17</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>9</v>
@@ -2487,10 +2492,10 @@
         <v>18</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>9</v>
@@ -2537,10 +2542,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>9</v>
@@ -2587,10 +2592,10 @@
         <v>20</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>9</v>
@@ -2637,10 +2642,10 @@
         <v>21</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>9</v>
@@ -2687,10 +2692,10 @@
         <v>22</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>9</v>
@@ -2737,10 +2742,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>9</v>
@@ -2787,10 +2792,10 @@
         <v>24</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>9</v>
@@ -2837,10 +2842,10 @@
         <v>25</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>9</v>
@@ -2887,10 +2892,10 @@
         <v>26</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>9</v>
@@ -2937,10 +2942,10 @@
         <v>27</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>9</v>
@@ -2987,10 +2992,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>9</v>
@@ -3037,10 +3042,10 @@
         <v>29</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>9</v>
@@ -3087,10 +3092,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>9</v>
@@ -3137,10 +3142,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>9</v>
@@ -3187,10 +3192,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>9</v>
@@ -3237,10 +3242,10 @@
         <v>33</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>9</v>
@@ -3287,10 +3292,10 @@
         <v>34</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>9</v>
@@ -3337,10 +3342,10 @@
         <v>35</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D41" s="25" t="s">
         <v>9</v>
@@ -3387,10 +3392,10 @@
         <v>36</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>9</v>
@@ -3437,10 +3442,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D43" s="25" t="s">
         <v>9</v>
@@ -3487,10 +3492,10 @@
         <v>38</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>9</v>
@@ -3537,10 +3542,10 @@
         <v>39</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>9</v>
@@ -3587,10 +3592,10 @@
         <v>40</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>9</v>
@@ -3637,10 +3642,10 @@
         <v>41</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>9</v>
@@ -3687,10 +3692,10 @@
         <v>42</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>9</v>
@@ -3737,10 +3742,10 @@
         <v>43</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>9</v>
@@ -3787,10 +3792,10 @@
         <v>44</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>9</v>
@@ -3837,10 +3842,10 @@
         <v>45</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D51" s="25" t="s">
         <v>9</v>
@@ -3887,10 +3892,10 @@
         <v>46</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>9</v>
@@ -3937,10 +3942,10 @@
         <v>47</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>9</v>
@@ -3987,10 +3992,10 @@
         <v>48</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>9</v>
@@ -4037,10 +4042,10 @@
         <v>49</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C55" s="33" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>9</v>
@@ -4087,10 +4092,10 @@
         <v>50</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>9</v>
@@ -4137,10 +4142,10 @@
         <v>51</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D57" s="25" t="s">
         <v>9</v>
@@ -4187,10 +4192,10 @@
         <v>52</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>9</v>
@@ -4237,10 +4242,10 @@
         <v>53</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>9</v>
@@ -4287,10 +4292,10 @@
         <v>54</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>9</v>
@@ -4337,10 +4342,10 @@
         <v>55</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>9</v>
@@ -4387,10 +4392,10 @@
         <v>56</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>9</v>
@@ -4437,10 +4442,10 @@
         <v>57</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C63" s="33" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D63" s="25" t="s">
         <v>9</v>
@@ -4487,10 +4492,10 @@
         <v>58</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C64" s="33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>9</v>
@@ -4537,10 +4542,10 @@
         <v>59</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D65" s="25" t="s">
         <v>9</v>
@@ -4587,10 +4592,10 @@
         <v>60</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>9</v>
@@ -4637,10 +4642,10 @@
         <v>61</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>9</v>
@@ -4687,10 +4692,10 @@
         <v>62</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>9</v>
@@ -4737,10 +4742,10 @@
         <v>63</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>9</v>
@@ -4787,10 +4792,10 @@
         <v>64</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>9</v>
@@ -4837,10 +4842,10 @@
         <v>65</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>9</v>
@@ -4887,10 +4892,10 @@
         <v>66</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C72" s="33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D72" s="25" t="s">
         <v>9</v>
@@ -4937,10 +4942,10 @@
         <v>67</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C73" s="33" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D73" s="25" t="s">
         <v>9</v>
@@ -4987,10 +4992,10 @@
         <v>68</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D74" s="25" t="s">
         <v>9</v>
@@ -5037,10 +5042,10 @@
         <v>69</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C75" s="33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D75" s="25" t="s">
         <v>9</v>
@@ -5087,10 +5092,10 @@
         <v>70</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C76" s="33" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D76" s="25" t="s">
         <v>9</v>
@@ -5137,10 +5142,10 @@
         <v>71</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>9</v>
@@ -5187,10 +5192,10 @@
         <v>72</v>
       </c>
       <c r="B78" s="32" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D78" s="25" t="s">
         <v>9</v>
@@ -5237,10 +5242,10 @@
         <v>73</v>
       </c>
       <c r="B79" s="32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D79" s="25" t="s">
         <v>9</v>
@@ -5287,10 +5292,10 @@
         <v>74</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C80" s="33" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D80" s="25" t="s">
         <v>9</v>
@@ -5337,10 +5342,10 @@
         <v>75</v>
       </c>
       <c r="B81" s="32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D81" s="25" t="s">
         <v>9</v>
@@ -5387,10 +5392,10 @@
         <v>76</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C82" s="33" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D82" s="25" t="s">
         <v>9</v>
@@ -5437,10 +5442,10 @@
         <v>77</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D83" s="25" t="s">
         <v>9</v>
@@ -5487,10 +5492,10 @@
         <v>78</v>
       </c>
       <c r="B84" s="32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C84" s="33" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D84" s="25" t="s">
         <v>9</v>
@@ -5537,10 +5542,10 @@
         <v>79</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C85" s="33" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D85" s="25" t="s">
         <v>9</v>
@@ -5587,10 +5592,10 @@
         <v>80</v>
       </c>
       <c r="B86" s="32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C86" s="33" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>9</v>

</xml_diff>